<commit_message>
change datatype for database
</commit_message>
<xml_diff>
--- a/static/employee_template.xlsx
+++ b/static/employee_template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\employee_form\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0776DA9-BC9B-4A09-AFDD-15BBF49AC987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA61B0D-5F2A-480F-9917-5312B7FB1250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -622,7 +622,7 @@
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -802,7 +802,7 @@
   <dimension ref="B2:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
adjust department&division and function
</commit_message>
<xml_diff>
--- a/static/employee_template.xlsx
+++ b/static/employee_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\employee_form\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E040C8A-8053-4B0F-A73C-FE448FF52709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC71899D-405B-4668-8674-6596A0BA7B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
   <si>
     <t>id</t>
   </si>
@@ -157,24 +157,12 @@
     <t>Advisory Division</t>
   </si>
   <si>
-    <t>BOM 1</t>
-  </si>
-  <si>
-    <t>BOM 2</t>
-  </si>
-  <si>
     <t>Brokerage Division</t>
   </si>
   <si>
-    <t>Company Secretariat</t>
-  </si>
-  <si>
     <t>Covered Warrant Division</t>
   </si>
   <si>
-    <t>Customer Care Center</t>
-  </si>
-  <si>
     <t>Dealing Division</t>
   </si>
   <si>
@@ -187,9 +175,6 @@
     <t>General Affairs Division</t>
   </si>
   <si>
-    <t>Human Resources Division</t>
-  </si>
-  <si>
     <t>Internal Control Division</t>
   </si>
   <si>
@@ -254,6 +239,45 @@
   </si>
   <si>
     <t>Business Support Department</t>
+  </si>
+  <si>
+    <t>Office Assistant Division</t>
+  </si>
+  <si>
+    <t>Company Secretariat Division</t>
+  </si>
+  <si>
+    <t>Internal Audit Division</t>
+  </si>
+  <si>
+    <t>People &amp; Workplace Division</t>
+  </si>
+  <si>
+    <t>Customer Care Department</t>
+  </si>
+  <si>
+    <t>Business Analysis(Function)</t>
+  </si>
+  <si>
+    <t>Workplace(Receptionist)</t>
+  </si>
+  <si>
+    <t>Consultant(Function)</t>
+  </si>
+  <si>
+    <t>Margin &amp; Settlement(Financial Product)</t>
+  </si>
+  <si>
+    <t>Margin &amp; Settlement (Operation)</t>
+  </si>
+  <si>
+    <t>Data Engineer(Function)</t>
+  </si>
+  <si>
+    <t>Workplace(Purchasing)</t>
+  </si>
+  <si>
+    <t>Workplace(General)</t>
   </si>
 </sst>
 </file>
@@ -309,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -317,6 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,7 +647,7 @@
   <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -770,13 +795,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBCC7BD9-C620-402D-B5D0-49F765AC353A}">
           <x14:formula1>
-            <xm:f>Sheet2!$C$2:$C$22</xm:f>
+            <xm:f>Sheet2!$C$2:$C$21</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE220895-8907-48C2-B791-FD391F681FD7}">
           <x14:formula1>
-            <xm:f>Sheet2!$D$2:$D$15</xm:f>
+            <xm:f>Sheet2!$D$2:$D$60</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F100</xm:sqref>
         </x14:dataValidation>
@@ -788,10 +813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -810,7 +835,7 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -823,8 +848,8 @@
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
-        <v>62</v>
+      <c r="D3" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -835,10 +860,10 @@
         <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
+        <v>71</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -849,10 +874,10 @@
         <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>67</v>
+        <v>43</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -863,10 +888,10 @@
         <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -877,10 +902,10 @@
         <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>64</v>
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.45">
@@ -888,101 +913,194 @@
         <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>65</v>
+        <v>73</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
+        <v>46</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
+        <v>47</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
+        <v>48</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
+        <v>49</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" t="s">
-        <v>75</v>
+        <v>50</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C20" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C17" s="2" t="s">
+      <c r="D20" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C21" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C18" s="2" t="s">
+      <c r="D21" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D22" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D23" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D24" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D48" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C19" s="2" t="s">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D49" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C20" s="2" t="s">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D51" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D52" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C21" s="2" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D53" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C22" s="2" t="s">
-        <v>61</v>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D60" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>